<commit_message>
Commit for TestBase Setup
</commit_message>
<xml_diff>
--- a/FacebookAutomation/Credentials.xlsx
+++ b/FacebookAutomation/Credentials.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\WebAppAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FacebookAutomation\FacebookAutomation\FacebookAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,7 +38,7 @@
     <t>Browser</t>
   </si>
   <si>
-    <t>Chrome</t>
+    <t>Firefox</t>
   </si>
   <si>
     <t>https://www.facebook.com/</t>

</xml_diff>

<commit_message>
Basic Setup for login
</commit_message>
<xml_diff>
--- a/FacebookAutomation/Credentials.xlsx
+++ b/FacebookAutomation/Credentials.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setupdetails" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>WebApplication Automation</t>
   </si>
@@ -42,6 +43,21 @@
   </si>
   <si>
     <t>https://www.facebook.com/</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>nivipriya1001@gmail.com</t>
+  </si>
+  <si>
+    <t>Lotica@123</t>
   </si>
 </sst>
 </file>
@@ -73,7 +89,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -83,6 +99,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -178,10 +200,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -195,6 +220,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -492,14 +526,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -510,7 +544,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -534,4 +568,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" customWidth="1"/>
+    <col min="3" max="3" width="43.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>